<commit_message>
Bulk Upload and OTP related Files
</commit_message>
<xml_diff>
--- a/public/download/product_bulk_demo.xlsx
+++ b/public/download/product_bulk_demo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ActiveIT Zone\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sites\ql28\public\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2362A731-E0D7-4E03-A113-90C9E6D93E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -53,18 +54,9 @@
     <t>pc</t>
   </si>
   <si>
-    <t>youtube</t>
-  </si>
-  <si>
     <t>slug</t>
   </si>
   <si>
-    <t>demo-product-22</t>
-  </si>
-  <si>
-    <t>Demo Product 22</t>
-  </si>
-  <si>
     <t>current_stock</t>
   </si>
   <si>
@@ -77,34 +69,76 @@
     <t>thumbnail_img</t>
   </si>
   <si>
-    <t>https://adyanmart.s3.ap-southeast-1.amazonaws.com/uploads/products/thumbnail/ZJqm0yHhBrLD7Zn2Wbtw6nkKxKtB9xntMh8ON8D1.jpeg</t>
-  </si>
-  <si>
     <t>photos</t>
   </si>
   <si>
-    <t>https://adyanmart.s3.ap-southeast-1.amazonaws.com/uploads/products/thumbnail/ZJqm0yHhBrLD7Zn2Wbtw6nkKxKtB9xntMh8ON8D1.jpeg,https://adyanmart.s3.ap-southeast-1.amazonaws.com/uploads/products/thumbnail/ZJqm0yHhBrLD7Zn2Wbtw6nkKxKtB9xntMh8ON8D1.jpeg</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
-    <t>Demo Product Description</t>
-  </si>
-  <si>
     <t>sku</t>
   </si>
   <si>
     <t>tags</t>
   </si>
   <si>
-    <t xml:space="preserve">Best Selling,demo Product,Baby product </t>
+    <t>returnable</t>
+  </si>
+  <si>
+    <t>returnable_days</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>discount_type</t>
+  </si>
+  <si>
+    <t>earn_point</t>
+  </si>
+  <si>
+    <t>expiry_month</t>
+  </si>
+  <si>
+    <t>expiry_year</t>
+  </si>
+  <si>
+    <t>batch_number</t>
+  </si>
+  <si>
+    <t>hsn_code</t>
+  </si>
+  <si>
+    <t>Demo Product 23</t>
+  </si>
+  <si>
+    <t>Demo Product Description 23</t>
+  </si>
+  <si>
+    <t>Demo, Baby</t>
+  </si>
+  <si>
+    <t>demo-product-23</t>
+  </si>
+  <si>
+    <t>SKU-23</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>BT-OCT22</t>
+  </si>
+  <si>
+    <t>HSN3029</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,36 +468,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="1" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="12" width="23.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="126.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="11" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="22" width="15.88671875" customWidth="1"/>
+    <col min="23" max="23" width="11.88671875" customWidth="1"/>
+    <col min="24" max="24" width="18.33203125" customWidth="1"/>
+    <col min="25" max="25" width="126.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -478,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -490,33 +524,60 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -524,43 +585,59 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H2">
-        <v>55</v>
+        <v>200</v>
       </c>
       <c r="I2">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="J2" t="s">
         <v>8</v>
       </c>
       <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>12</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2">
         <v>11</v>
       </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2">
+        <v>2023</v>
+      </c>
+      <c r="U2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1"/>
-    <hyperlink ref="Q2" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bulk upload excel update
</commit_message>
<xml_diff>
--- a/public/download/product_bulk_demo.xlsx
+++ b/public/download/product_bulk_demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sites\ql28\public\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01 Assignments\Steve\Quicklabs\backup\23-Nov-2022\from Live Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2362A731-E0D7-4E03-A113-90C9E6D93E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B63DC4-C558-4C6B-9832-29136EE4892D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="2688" windowWidth="21240" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
   <si>
     <t>category_id</t>
-  </si>
-  <si>
-    <t>brand_id</t>
   </si>
   <si>
     <t>video_provider</t>
@@ -469,35 +466,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" customWidth="1"/>
-    <col min="6" max="7" width="16.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1"/>
-    <col min="11" max="12" width="23.6640625" customWidth="1"/>
-    <col min="13" max="22" width="15.88671875" customWidth="1"/>
-    <col min="23" max="23" width="11.88671875" customWidth="1"/>
-    <col min="24" max="24" width="18.33203125" customWidth="1"/>
-    <col min="25" max="25" width="126.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="11" width="23.6640625" customWidth="1"/>
+    <col min="12" max="21" width="15.88671875" customWidth="1"/>
+    <col min="22" max="22" width="11.88671875" customWidth="1"/>
+    <col min="23" max="23" width="18.33203125" customWidth="1"/>
+    <col min="24" max="24" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -509,10 +505,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -521,16 +517,16 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>18</v>
@@ -557,7 +553,7 @@
         <v>25</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>11</v>
@@ -568,73 +564,67 @@
       <c r="Y1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <v>200</v>
+      </c>
+      <c r="H2">
+        <v>120</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2">
-        <v>200</v>
-      </c>
-      <c r="I2">
-        <v>120</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2">
-        <v>35</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2" t="s">
         <v>31</v>
       </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>12</v>
-      </c>
-      <c r="P2">
-        <v>10</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="Q2">
+        <v>11</v>
+      </c>
+      <c r="R2" t="s">
         <v>32</v>
       </c>
-      <c r="R2">
-        <v>11</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="S2">
+        <v>2023</v>
+      </c>
+      <c r="T2" t="s">
         <v>33</v>
-      </c>
-      <c r="T2">
-        <v>2023</v>
       </c>
       <c r="U2" t="s">
         <v>34</v>
       </c>
-      <c r="V2" t="s">
-        <v>35</v>
-      </c>
+      <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating bulk upload excel sheet
</commit_message>
<xml_diff>
--- a/public/download/product_bulk_demo.xlsx
+++ b/public/download/product_bulk_demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01 Assignments\Steve\Quicklabs\backup\23-Nov-2022\from Live Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sampa\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B63DC4-C558-4C6B-9832-29136EE4892D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB8E63D-3689-441D-814D-8BC7D53C1857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="2688" windowWidth="21240" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="21240" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>HSN3029</t>
+  </si>
+  <si>
+    <t>brand_id</t>
   </si>
 </sst>
 </file>
@@ -466,29 +469,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="6" width="16.5546875" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="11" width="23.6640625" customWidth="1"/>
-    <col min="12" max="21" width="15.88671875" customWidth="1"/>
-    <col min="22" max="22" width="11.88671875" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" customWidth="1"/>
-    <col min="24" max="24" width="27.21875" customWidth="1"/>
+    <col min="3" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="11" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="22" width="15.88671875" customWidth="1"/>
+    <col min="23" max="23" width="11.88671875" customWidth="1"/>
+    <col min="24" max="24" width="18.33203125" customWidth="1"/>
+    <col min="25" max="25" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,73 +502,76 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -575,56 +581,59 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>200</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>120</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>35</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>30</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>12</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>10</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>11</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>32</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>2023</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>33</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>